<commit_message>
add the FILI Sheet as removed space
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Client/FILI.xlsx
+++ b/src/test/resources/testdata/Client/FILI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CE5437-FEEB-4A60-91ED-9C39BEBB62D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70B0153-9E32-485E-8DA7-22DFE75EA5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" activeTab="5" xr2:uid="{8D0F94DE-3100-47E5-A17C-DB8B711FEBE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="731" activeTab="5" xr2:uid="{8D0F94DE-3100-47E5-A17C-DB8B711FEBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision &amp; Admin" sheetId="6" r:id="rId1"/>
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9885" uniqueCount="2405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9885" uniqueCount="2406">
   <si>
     <t>Version</t>
   </si>
@@ -10804,6 +10804,9 @@
   </si>
   <si>
     <t>If InheritedNQ_Payment_WithholdFederal_Tax_Percentage= Blank, then ISSUE ERROR MESSAGE: Percentage is required.</t>
+  </si>
+  <si>
+    <t>If InheritedNQ_Payment_WithholdStateTax_Amount = Blank AND InheritedNQ_Payment_WithholdStateTax_Percentage = Blank, then ISSUE ERROR MESSAGE: Amount or Percentage is required.</t>
   </si>
 </sst>
 </file>
@@ -29933,9 +29936,9 @@
   <dimension ref="A1:AZ205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AE100" sqref="AE100"/>
+      <selection pane="bottomLeft" activeCell="AH98" sqref="AH98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="104.25" customHeight="1"/>
@@ -41677,7 +41680,7 @@
         <v>2392</v>
       </c>
       <c r="AI99" s="151" t="s">
-        <v>2387</v>
+        <v>2405</v>
       </c>
       <c r="AJ99" s="110"/>
       <c r="AK99" s="508" t="s">

</xml_diff>

<commit_message>
FILI_WizardTest2103 : Code pushed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Client/FILI.xlsx
+++ b/src/test/resources/testdata/Client/FILI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70B0153-9E32-485E-8DA7-22DFE75EA5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CA4143-F56A-413A-8D58-F37B0FC6E0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="731" activeTab="5" xr2:uid="{8D0F94DE-3100-47E5-A17C-DB8B711FEBE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" activeTab="5" xr2:uid="{8D0F94DE-3100-47E5-A17C-DB8B711FEBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision &amp; Admin" sheetId="6" r:id="rId1"/>
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9885" uniqueCount="2406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9885" uniqueCount="2405">
   <si>
     <t>Version</t>
   </si>
@@ -10742,9 +10742,6 @@
   </si>
   <si>
     <t>If InheritedNQ_Payment_WithholdState Tax_YesNo= Blank, then ISSUE ERROR MESSAGE: Please Select Yes or No.</t>
-  </si>
-  <si>
-    <t>If InheritedNQ_Payment_WithholdState Tax_Amount = Blank AND InheritedNQ_Payment_WithholdStateTax_Percentage = Blank, then ISSUE ERROR MESSAGE: Amount or Percentage is required.</t>
   </si>
   <si>
     <t>Annuity_TaxQualification = Inherited Non-Qualified</t>
@@ -14946,17 +14943,17 @@
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
     <col min="9" max="9" width="35" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" customWidth="1"/>
+    <col min="11" max="11" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:11" ht="28.8">
       <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
@@ -14984,7 +14981,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30">
+    <row r="2" spans="1:11" ht="28.8">
       <c r="A2" s="251">
         <v>0</v>
       </c>
@@ -15006,7 +15003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45">
+    <row r="3" spans="1:11" ht="43.2">
       <c r="A3" s="86">
         <v>0.1</v>
       </c>
@@ -15028,7 +15025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:11" ht="28.8">
       <c r="A4" s="86">
         <v>0.1</v>
       </c>
@@ -15050,7 +15047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="270">
+    <row r="5" spans="1:11" ht="230.4">
       <c r="A5" s="86">
         <v>0.1</v>
       </c>
@@ -15068,7 +15065,7 @@
       </c>
       <c r="F5" s="86"/>
     </row>
-    <row r="6" spans="1:11" ht="90">
+    <row r="6" spans="1:11" ht="72">
       <c r="A6" s="86">
         <v>0.2</v>
       </c>
@@ -15086,7 +15083,7 @@
       </c>
       <c r="F6" s="86"/>
     </row>
-    <row r="7" spans="1:11" ht="30">
+    <row r="7" spans="1:11" ht="28.8">
       <c r="A7" s="86">
         <v>0.2</v>
       </c>
@@ -15122,7 +15119,7 @@
       </c>
       <c r="F8" s="86"/>
     </row>
-    <row r="9" spans="1:11" ht="75">
+    <row r="9" spans="1:11" ht="57.6">
       <c r="A9" s="86">
         <v>0.3</v>
       </c>
@@ -15160,7 +15157,7 @@
       </c>
       <c r="F10" s="86"/>
     </row>
-    <row r="11" spans="1:11" ht="75">
+    <row r="11" spans="1:11" ht="57.6">
       <c r="A11" s="86">
         <v>0.4</v>
       </c>
@@ -15178,7 +15175,7 @@
       </c>
       <c r="F11" s="86"/>
     </row>
-    <row r="12" spans="1:11" ht="30">
+    <row r="12" spans="1:11" ht="28.8">
       <c r="A12" s="86">
         <v>0.4</v>
       </c>
@@ -15196,7 +15193,7 @@
       </c>
       <c r="F12" s="86"/>
     </row>
-    <row r="13" spans="1:11" ht="60">
+    <row r="13" spans="1:11" ht="57.6">
       <c r="A13" s="86">
         <v>0.4</v>
       </c>
@@ -15214,7 +15211,7 @@
       </c>
       <c r="F13" s="86"/>
     </row>
-    <row r="14" spans="1:11" ht="195">
+    <row r="14" spans="1:11" ht="172.8">
       <c r="A14" s="86">
         <v>0.4</v>
       </c>
@@ -15232,7 +15229,7 @@
       </c>
       <c r="F14" s="86"/>
     </row>
-    <row r="15" spans="1:11" ht="90">
+    <row r="15" spans="1:11" ht="72">
       <c r="A15" s="86">
         <v>0.4</v>
       </c>
@@ -15268,7 +15265,7 @@
       </c>
       <c r="F16" s="86"/>
     </row>
-    <row r="17" spans="1:6" ht="105">
+    <row r="17" spans="1:6" ht="72">
       <c r="A17" s="86">
         <v>0.4</v>
       </c>
@@ -15286,7 +15283,7 @@
       </c>
       <c r="F17" s="86"/>
     </row>
-    <row r="18" spans="1:6" ht="30">
+    <row r="18" spans="1:6" ht="28.8">
       <c r="A18" s="86">
         <v>0.4</v>
       </c>
@@ -15304,7 +15301,7 @@
       </c>
       <c r="F18" s="86"/>
     </row>
-    <row r="19" spans="1:6" ht="105">
+    <row r="19" spans="1:6" ht="86.4">
       <c r="A19" s="86">
         <v>0.4</v>
       </c>
@@ -15322,7 +15319,7 @@
       </c>
       <c r="F19" s="86"/>
     </row>
-    <row r="20" spans="1:6" ht="75">
+    <row r="20" spans="1:6" ht="57.6">
       <c r="A20" s="86">
         <v>0.5</v>
       </c>
@@ -15340,7 +15337,7 @@
       </c>
       <c r="F20" s="86"/>
     </row>
-    <row r="21" spans="1:6" ht="90">
+    <row r="21" spans="1:6" ht="72">
       <c r="A21" s="86">
         <v>0.5</v>
       </c>
@@ -15358,7 +15355,7 @@
       </c>
       <c r="F21" s="86"/>
     </row>
-    <row r="22" spans="1:6" ht="195">
+    <row r="22" spans="1:6" ht="187.2">
       <c r="A22" s="86">
         <v>0.5</v>
       </c>
@@ -15376,7 +15373,7 @@
       </c>
       <c r="F22" s="86"/>
     </row>
-    <row r="23" spans="1:6" ht="45">
+    <row r="23" spans="1:6" ht="43.2">
       <c r="A23" s="86">
         <v>0.5</v>
       </c>
@@ -15394,7 +15391,7 @@
       </c>
       <c r="F23" s="86"/>
     </row>
-    <row r="24" spans="1:6" ht="30">
+    <row r="24" spans="1:6" ht="28.8">
       <c r="A24" s="86">
         <v>0.5</v>
       </c>
@@ -15412,7 +15409,7 @@
       </c>
       <c r="F24" s="86"/>
     </row>
-    <row r="25" spans="1:6" ht="90">
+    <row r="25" spans="1:6" ht="72">
       <c r="A25" s="86">
         <v>0.6</v>
       </c>
@@ -15430,7 +15427,7 @@
       </c>
       <c r="F25" s="86"/>
     </row>
-    <row r="26" spans="1:6" ht="285">
+    <row r="26" spans="1:6" ht="244.8">
       <c r="A26" s="86">
         <v>0.6</v>
       </c>
@@ -15448,7 +15445,7 @@
       </c>
       <c r="F26" s="86"/>
     </row>
-    <row r="27" spans="1:6" ht="120">
+    <row r="27" spans="1:6" ht="100.8">
       <c r="A27" s="86">
         <v>0.6</v>
       </c>
@@ -15466,7 +15463,7 @@
       </c>
       <c r="F27" s="86"/>
     </row>
-    <row r="28" spans="1:6" ht="120">
+    <row r="28" spans="1:6" ht="115.2">
       <c r="A28" s="86">
         <v>0.6</v>
       </c>
@@ -15484,7 +15481,7 @@
       </c>
       <c r="F28" s="86"/>
     </row>
-    <row r="29" spans="1:6" ht="75">
+    <row r="29" spans="1:6" ht="57.6">
       <c r="A29" s="86">
         <v>0.6</v>
       </c>
@@ -15502,7 +15499,7 @@
       </c>
       <c r="F29" s="86"/>
     </row>
-    <row r="30" spans="1:6" ht="45">
+    <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="86">
         <v>0.6</v>
       </c>
@@ -15520,7 +15517,7 @@
       </c>
       <c r="F30" s="86"/>
     </row>
-    <row r="31" spans="1:6" ht="105">
+    <row r="31" spans="1:6" ht="86.4">
       <c r="A31" s="86">
         <v>0.7</v>
       </c>
@@ -15538,7 +15535,7 @@
       </c>
       <c r="F31" s="86"/>
     </row>
-    <row r="32" spans="1:6" ht="60">
+    <row r="32" spans="1:6" ht="57.6">
       <c r="A32" s="86">
         <v>0.7</v>
       </c>
@@ -15556,7 +15553,7 @@
       </c>
       <c r="F32" s="86"/>
     </row>
-    <row r="33" spans="1:6" ht="45">
+    <row r="33" spans="1:6" ht="28.8">
       <c r="A33" s="86">
         <v>0.7</v>
       </c>
@@ -15574,7 +15571,7 @@
       </c>
       <c r="F33" s="86"/>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="86">
         <v>0.7</v>
       </c>
@@ -15592,7 +15589,7 @@
       </c>
       <c r="F34" s="86"/>
     </row>
-    <row r="35" spans="1:6" ht="45">
+    <row r="35" spans="1:6" ht="28.8">
       <c r="A35" s="86">
         <v>0.8</v>
       </c>
@@ -15610,7 +15607,7 @@
       </c>
       <c r="F35" s="86"/>
     </row>
-    <row r="36" spans="1:6" ht="105">
+    <row r="36" spans="1:6" ht="86.4">
       <c r="A36" s="86">
         <v>0.8</v>
       </c>
@@ -15628,7 +15625,7 @@
       </c>
       <c r="F36" s="86"/>
     </row>
-    <row r="37" spans="1:6" ht="255">
+    <row r="37" spans="1:6" ht="230.4">
       <c r="A37" s="86">
         <v>0.8</v>
       </c>
@@ -15646,7 +15643,7 @@
       </c>
       <c r="F37" s="86"/>
     </row>
-    <row r="38" spans="1:6" ht="60">
+    <row r="38" spans="1:6" ht="57.6">
       <c r="A38" s="86">
         <v>0.8</v>
       </c>
@@ -15664,7 +15661,7 @@
       </c>
       <c r="F38" s="86"/>
     </row>
-    <row r="39" spans="1:6" ht="45">
+    <row r="39" spans="1:6" ht="43.2">
       <c r="A39" s="86">
         <v>0.8</v>
       </c>
@@ -15682,7 +15679,7 @@
       </c>
       <c r="F39" s="86"/>
     </row>
-    <row r="40" spans="1:6" ht="75">
+    <row r="40" spans="1:6" ht="57.6">
       <c r="A40" s="86">
         <v>0.8</v>
       </c>
@@ -15700,7 +15697,7 @@
       </c>
       <c r="F40" s="86"/>
     </row>
-    <row r="41" spans="1:6" ht="30">
+    <row r="41" spans="1:6" ht="28.8">
       <c r="A41" s="86">
         <v>0.8</v>
       </c>
@@ -15718,7 +15715,7 @@
       </c>
       <c r="F41" s="86"/>
     </row>
-    <row r="42" spans="1:6" ht="30">
+    <row r="42" spans="1:6" ht="28.8">
       <c r="A42" s="86">
         <v>0.8</v>
       </c>
@@ -15736,7 +15733,7 @@
       </c>
       <c r="F42" s="86"/>
     </row>
-    <row r="43" spans="1:6" ht="45">
+    <row r="43" spans="1:6" ht="43.2">
       <c r="A43" s="86">
         <v>0.8</v>
       </c>
@@ -15754,7 +15751,7 @@
       </c>
       <c r="F43" s="86"/>
     </row>
-    <row r="44" spans="1:6" ht="30">
+    <row r="44" spans="1:6" ht="28.8">
       <c r="A44" s="86">
         <v>0.8</v>
       </c>
@@ -15772,7 +15769,7 @@
       </c>
       <c r="F44" s="86"/>
     </row>
-    <row r="45" spans="1:6" ht="165">
+    <row r="45" spans="1:6" ht="144">
       <c r="A45" s="86">
         <v>0.8</v>
       </c>
@@ -15790,7 +15787,7 @@
       </c>
       <c r="F45" s="86"/>
     </row>
-    <row r="46" spans="1:6" ht="30">
+    <row r="46" spans="1:6" ht="28.8">
       <c r="A46" s="86">
         <v>0.8</v>
       </c>
@@ -15808,7 +15805,7 @@
       </c>
       <c r="F46" s="86"/>
     </row>
-    <row r="47" spans="1:6" ht="135">
+    <row r="47" spans="1:6" ht="100.8">
       <c r="A47" s="86">
         <v>0.8</v>
       </c>
@@ -15826,7 +15823,7 @@
       </c>
       <c r="F47" s="86"/>
     </row>
-    <row r="48" spans="1:6" ht="30">
+    <row r="48" spans="1:6" ht="28.8">
       <c r="A48" s="86">
         <v>0.9</v>
       </c>
@@ -15844,7 +15841,7 @@
       </c>
       <c r="F48" s="86"/>
     </row>
-    <row r="49" spans="1:6" ht="120">
+    <row r="49" spans="1:6" ht="100.8">
       <c r="A49" s="86">
         <v>0.9</v>
       </c>
@@ -15862,7 +15859,7 @@
       </c>
       <c r="F49" s="86"/>
     </row>
-    <row r="50" spans="1:6" ht="60">
+    <row r="50" spans="1:6" ht="57.6">
       <c r="A50" s="86">
         <v>0.9</v>
       </c>
@@ -15880,7 +15877,7 @@
       </c>
       <c r="F50" s="86"/>
     </row>
-    <row r="51" spans="1:6" ht="45">
+    <row r="51" spans="1:6" ht="28.8">
       <c r="A51" s="86">
         <v>0.9</v>
       </c>
@@ -15898,7 +15895,7 @@
       </c>
       <c r="F51" s="86"/>
     </row>
-    <row r="52" spans="1:6" ht="60">
+    <row r="52" spans="1:6" ht="43.2">
       <c r="A52" s="450">
         <v>0.1</v>
       </c>
@@ -15916,7 +15913,7 @@
       </c>
       <c r="F52" s="86"/>
     </row>
-    <row r="53" spans="1:6" ht="150">
+    <row r="53" spans="1:6" ht="115.2">
       <c r="A53" s="450">
         <v>0.1</v>
       </c>
@@ -15934,7 +15931,7 @@
       </c>
       <c r="F53" s="86"/>
     </row>
-    <row r="54" spans="1:6" ht="30">
+    <row r="54" spans="1:6" ht="28.8">
       <c r="A54" s="450">
         <v>0.1</v>
       </c>
@@ -15952,7 +15949,7 @@
       </c>
       <c r="F54" s="86"/>
     </row>
-    <row r="55" spans="1:6" ht="270">
+    <row r="55" spans="1:6" ht="216">
       <c r="A55" s="450">
         <v>0.1</v>
       </c>
@@ -15970,7 +15967,7 @@
       </c>
       <c r="F55" s="86"/>
     </row>
-    <row r="56" spans="1:6" ht="255">
+    <row r="56" spans="1:6" ht="216">
       <c r="A56" s="450">
         <v>0.1</v>
       </c>
@@ -15988,7 +15985,7 @@
       </c>
       <c r="F56" s="86"/>
     </row>
-    <row r="57" spans="1:6" ht="45">
+    <row r="57" spans="1:6" ht="43.2">
       <c r="A57" s="450">
         <v>0.1</v>
       </c>
@@ -16006,7 +16003,7 @@
       </c>
       <c r="F57" s="86"/>
     </row>
-    <row r="58" spans="1:6" ht="105">
+    <row r="58" spans="1:6" ht="86.4">
       <c r="A58" s="450">
         <v>0.1</v>
       </c>
@@ -16024,7 +16021,7 @@
       </c>
       <c r="F58" s="86"/>
     </row>
-    <row r="59" spans="1:6" ht="30">
+    <row r="59" spans="1:6" ht="28.8">
       <c r="A59" s="450">
         <v>0.1</v>
       </c>
@@ -16042,7 +16039,7 @@
       </c>
       <c r="F59" s="86"/>
     </row>
-    <row r="60" spans="1:6" ht="30">
+    <row r="60" spans="1:6" ht="28.8">
       <c r="A60" s="450">
         <v>0.1</v>
       </c>
@@ -16060,7 +16057,7 @@
       </c>
       <c r="F60" s="86"/>
     </row>
-    <row r="61" spans="1:6" ht="120">
+    <row r="61" spans="1:6" ht="115.2">
       <c r="A61" s="450">
         <v>0.1</v>
       </c>
@@ -16078,7 +16075,7 @@
       </c>
       <c r="F61" s="86"/>
     </row>
-    <row r="62" spans="1:6" ht="105">
+    <row r="62" spans="1:6" ht="86.4">
       <c r="A62" s="450">
         <v>0.1</v>
       </c>
@@ -16114,7 +16111,7 @@
       </c>
       <c r="F63" s="86"/>
     </row>
-    <row r="64" spans="1:6" ht="30">
+    <row r="64" spans="1:6" ht="28.8">
       <c r="A64" s="450">
         <v>0.1</v>
       </c>
@@ -16142,7 +16139,7 @@
       <c r="E65" s="511"/>
       <c r="F65" s="86"/>
     </row>
-    <row r="66" spans="1:6" ht="30">
+    <row r="66" spans="1:6" ht="28.8">
       <c r="A66" s="470">
         <v>0.11</v>
       </c>
@@ -16159,7 +16156,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="45">
+    <row r="67" spans="1:6" ht="28.8">
       <c r="A67" s="470">
         <v>0.11</v>
       </c>
@@ -16176,7 +16173,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="30">
+    <row r="68" spans="1:6" ht="28.8">
       <c r="A68" s="470">
         <v>0.11</v>
       </c>
@@ -16193,7 +16190,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="30">
+    <row r="69" spans="1:6" ht="28.8">
       <c r="A69" s="470">
         <v>0.11</v>
       </c>
@@ -16230,16 +16227,16 @@
       <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45">
+    <row r="1" spans="1:5" ht="28.8">
       <c r="A1" s="191" t="s">
         <v>1530</v>
       </c>
@@ -16592,7 +16589,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30">
+    <row r="35" spans="1:10" ht="28.8">
       <c r="A35" s="86" t="s">
         <v>967</v>
       </c>
@@ -16783,45 +16780,45 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.140625" customWidth="1"/>
-    <col min="27" max="27" width="3.85546875" customWidth="1"/>
-    <col min="28" max="28" width="3.5703125" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.109375" customWidth="1"/>
+    <col min="27" max="27" width="3.88671875" customWidth="1"/>
+    <col min="28" max="28" width="3.5546875" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="52" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="66.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="66.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="32" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="52" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="52" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:270" s="24" customFormat="1" ht="24">
@@ -17154,7 +17151,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="5" spans="1:270" ht="120">
+    <row r="5" spans="1:270" ht="86.4">
       <c r="A5" s="186" t="s">
         <v>1557</v>
       </c>
@@ -17259,7 +17256,7 @@
       <c r="AZ5" s="86"/>
       <c r="BA5" s="86"/>
     </row>
-    <row r="6" spans="1:270" s="75" customFormat="1" ht="75">
+    <row r="6" spans="1:270" s="75" customFormat="1" ht="72">
       <c r="A6" s="186" t="s">
         <v>1557</v>
       </c>
@@ -17342,7 +17339,7 @@
       <c r="AZ6" s="185"/>
       <c r="BA6" s="185"/>
     </row>
-    <row r="7" spans="1:270" ht="45">
+    <row r="7" spans="1:270" ht="43.2">
       <c r="A7" s="186" t="s">
         <v>1557</v>
       </c>
@@ -17447,7 +17444,7 @@
       <c r="AZ7" s="86"/>
       <c r="BA7" s="86"/>
     </row>
-    <row r="8" spans="1:270" ht="45">
+    <row r="8" spans="1:270" ht="43.2">
       <c r="A8" s="186" t="s">
         <v>1557</v>
       </c>
@@ -17552,7 +17549,7 @@
       <c r="AZ8" s="86"/>
       <c r="BA8" s="86"/>
     </row>
-    <row r="9" spans="1:270" s="173" customFormat="1" ht="45">
+    <row r="9" spans="1:270" s="173" customFormat="1" ht="43.2">
       <c r="A9" s="186" t="s">
         <v>1557</v>
       </c>
@@ -17888,7 +17885,7 @@
       <c r="JI9"/>
       <c r="JJ9"/>
     </row>
-    <row r="10" spans="1:270" s="173" customFormat="1" ht="90">
+    <row r="10" spans="1:270" s="173" customFormat="1" ht="86.4">
       <c r="A10" s="186" t="s">
         <v>1557</v>
       </c>
@@ -18224,7 +18221,7 @@
       <c r="JI10"/>
       <c r="JJ10"/>
     </row>
-    <row r="11" spans="1:270" s="173" customFormat="1" ht="90">
+    <row r="11" spans="1:270" s="173" customFormat="1" ht="57.6">
       <c r="A11" s="186" t="s">
         <v>1557</v>
       </c>
@@ -18560,7 +18557,7 @@
       <c r="JI11"/>
       <c r="JJ11"/>
     </row>
-    <row r="12" spans="1:270" s="173" customFormat="1" ht="45">
+    <row r="12" spans="1:270" s="173" customFormat="1" ht="43.2">
       <c r="A12" s="186" t="s">
         <v>1557</v>
       </c>
@@ -18894,7 +18891,7 @@
       <c r="JI12"/>
       <c r="JJ12"/>
     </row>
-    <row r="13" spans="1:270" s="173" customFormat="1" ht="90">
+    <row r="13" spans="1:270" s="173" customFormat="1" ht="86.4">
       <c r="A13" s="186" t="s">
         <v>1557</v>
       </c>
@@ -19234,7 +19231,7 @@
       <c r="JI13"/>
       <c r="JJ13"/>
     </row>
-    <row r="14" spans="1:270" s="173" customFormat="1" ht="135">
+    <row r="14" spans="1:270" s="173" customFormat="1" ht="129.6">
       <c r="A14" s="186" t="s">
         <v>1557</v>
       </c>
@@ -19574,7 +19571,7 @@
       <c r="JI14"/>
       <c r="JJ14"/>
     </row>
-    <row r="15" spans="1:270" s="173" customFormat="1" ht="45">
+    <row r="15" spans="1:270" s="173" customFormat="1" ht="43.2">
       <c r="A15" s="186" t="s">
         <v>1557</v>
       </c>
@@ -19906,7 +19903,7 @@
       <c r="JI15"/>
       <c r="JJ15"/>
     </row>
-    <row r="16" spans="1:270" s="173" customFormat="1" ht="120">
+    <row r="16" spans="1:270" s="173" customFormat="1" ht="86.4">
       <c r="A16" s="186" t="s">
         <v>1557</v>
       </c>
@@ -20240,7 +20237,7 @@
       <c r="JI16"/>
       <c r="JJ16"/>
     </row>
-    <row r="17" spans="1:270" s="173" customFormat="1" ht="120">
+    <row r="17" spans="1:270" s="173" customFormat="1" ht="86.4">
       <c r="A17" s="186" t="s">
         <v>1557</v>
       </c>
@@ -20662,15 +20659,15 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="85.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" customWidth="1"/>
+    <col min="3" max="3" width="85.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -20699,7 +20696,7 @@
         <v>1606</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
+    <row r="2" spans="1:8" ht="28.8">
       <c r="A2" t="s">
         <v>1607</v>
       </c>
@@ -20765,7 +20762,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:8" ht="43.2">
       <c r="A9" t="s">
         <v>1611</v>
       </c>
@@ -20798,7 +20795,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="28.8">
       <c r="A12" t="s">
         <v>1616</v>
       </c>
@@ -20809,7 +20806,7 @@
         <v>1618</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30">
+    <row r="13" spans="1:8" ht="28.8">
       <c r="A13" t="s">
         <v>1616</v>
       </c>
@@ -20820,7 +20817,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="28.8">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -20831,7 +20828,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30">
+    <row r="15" spans="1:8" ht="28.8">
       <c r="B15" s="81" t="s">
         <v>1621</v>
       </c>
@@ -20839,7 +20836,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60">
+    <row r="16" spans="1:8" ht="57.6">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -20850,7 +20847,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="105">
+    <row r="17" spans="1:3" ht="100.8">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -20908,7 +20905,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24.75">
+    <row r="23" spans="1:3" ht="26.4">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -20928,7 +20925,7 @@
       </c>
       <c r="C24" s="160"/>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -20937,7 +20934,7 @@
       </c>
       <c r="C25" s="160"/>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="28.8">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -20957,7 +20954,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -20975,7 +20972,7 @@
       </c>
       <c r="C29" s="160"/>
     </row>
-    <row r="30" spans="1:3" ht="30">
+    <row r="30" spans="1:3" ht="28.8">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -20984,7 +20981,7 @@
       </c>
       <c r="C30" s="160"/>
     </row>
-    <row r="31" spans="1:3" ht="30">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -20993,7 +20990,7 @@
       </c>
       <c r="C31" s="160"/>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="28.8">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -21020,7 +21017,7 @@
       </c>
       <c r="C34" s="160"/>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -21029,7 +21026,7 @@
       </c>
       <c r="C35" s="160"/>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>1630</v>
       </c>
@@ -21040,7 +21037,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>1630</v>
       </c>
@@ -21051,7 +21048,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>1630</v>
       </c>
@@ -21062,7 +21059,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>1630</v>
       </c>
@@ -21073,7 +21070,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="28.8">
       <c r="A40" t="s">
         <v>1632</v>
       </c>
@@ -21084,7 +21081,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>1632</v>
       </c>
@@ -21128,7 +21125,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45">
+    <row r="45" spans="1:3" ht="43.2">
       <c r="A45" t="s">
         <v>1638</v>
       </c>
@@ -21139,7 +21136,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30">
+    <row r="46" spans="1:3" ht="28.8">
       <c r="A46" t="s">
         <v>1638</v>
       </c>
@@ -21177,20 +21174,20 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="24" customFormat="1" ht="48">
@@ -21248,7 +21245,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30">
+    <row r="3" spans="1:14" ht="28.8">
       <c r="A3" t="s">
         <v>982</v>
       </c>
@@ -21303,7 +21300,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30">
+    <row r="8" spans="1:14" ht="28.8">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -21325,7 +21322,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30">
+    <row r="10" spans="1:14" ht="28.8">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -21360,7 +21357,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="45">
+    <row r="13" spans="1:14" ht="43.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -21372,7 +21369,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="45">
+    <row r="14" spans="1:14" ht="43.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -21384,7 +21381,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="45">
+    <row r="15" spans="1:14" ht="43.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -21396,7 +21393,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="45">
+    <row r="16" spans="1:14" ht="43.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -21507,7 +21504,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="28.8">
       <c r="A26" t="s">
         <v>1692</v>
       </c>
@@ -21574,10 +21571,10 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="51.75" customHeight="1">
@@ -21824,7 +21821,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="69" t="s">
@@ -21862,9 +21859,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:53" s="24" customFormat="1" ht="54.95" customHeight="1">
+    <row r="1" spans="1:53" s="24" customFormat="1" ht="54.9" customHeight="1">
       <c r="A1" s="25"/>
       <c r="B1" s="26"/>
       <c r="C1" s="27" t="s">
@@ -22337,12 +22334,12 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5546875" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="56.1" customHeight="1">
@@ -22438,14 +22435,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21">
@@ -22688,7 +22685,7 @@
       </c>
       <c r="K8" s="154"/>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:12" ht="28.8">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -22722,7 +22719,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60">
+    <row r="10" spans="1:12" ht="43.2">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -22951,72 +22948,72 @@
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="261" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" style="261" customWidth="1"/>
     <col min="2" max="2" width="22" style="261" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="261" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="261" customWidth="1"/>
     <col min="4" max="4" width="14" style="261" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="261" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="261" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="261" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="261" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="261" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="262" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="261" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="261" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="261" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" style="261" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" style="261" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="261" customWidth="1"/>
-    <col min="17" max="18" width="14.42578125" style="262" customWidth="1"/>
-    <col min="19" max="19" width="25.5703125" style="261" customWidth="1"/>
-    <col min="20" max="20" width="21.5703125" style="261" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="261" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" style="261" customWidth="1"/>
-    <col min="23" max="26" width="14.42578125" style="261" customWidth="1"/>
-    <col min="27" max="27" width="19.140625" style="261" customWidth="1"/>
-    <col min="28" max="28" width="17.42578125" style="261" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" style="261" customWidth="1"/>
-    <col min="30" max="30" width="19.42578125" style="261" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" style="261" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" style="368" customWidth="1"/>
-    <col min="33" max="33" width="22.42578125" style="261" customWidth="1"/>
-    <col min="34" max="34" width="12.5703125" style="261" customWidth="1"/>
-    <col min="35" max="35" width="18.42578125" style="262" customWidth="1"/>
-    <col min="36" max="36" width="20.85546875" style="261" customWidth="1"/>
-    <col min="37" max="37" width="12.85546875" style="261" customWidth="1"/>
-    <col min="38" max="38" width="13.5703125" style="261" customWidth="1"/>
-    <col min="39" max="39" width="16.5703125" style="261" customWidth="1"/>
-    <col min="40" max="40" width="13.85546875" style="261" customWidth="1"/>
-    <col min="41" max="41" width="19.140625" style="261" customWidth="1"/>
-    <col min="42" max="42" width="16.5703125" style="261" customWidth="1"/>
-    <col min="43" max="43" width="14.5703125" style="261" customWidth="1"/>
-    <col min="44" max="44" width="14.85546875" style="261" customWidth="1"/>
-    <col min="45" max="45" width="15.42578125" style="261" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="261" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="261" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="261" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" style="261" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="261" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" style="262" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="261" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" style="261" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="261" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" style="261" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" style="261" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="261" customWidth="1"/>
+    <col min="17" max="18" width="14.44140625" style="262" customWidth="1"/>
+    <col min="19" max="19" width="25.5546875" style="261" customWidth="1"/>
+    <col min="20" max="20" width="21.5546875" style="261" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" style="261" customWidth="1"/>
+    <col min="22" max="22" width="19.5546875" style="261" customWidth="1"/>
+    <col min="23" max="26" width="14.44140625" style="261" customWidth="1"/>
+    <col min="27" max="27" width="19.109375" style="261" customWidth="1"/>
+    <col min="28" max="28" width="17.44140625" style="261" customWidth="1"/>
+    <col min="29" max="29" width="19.5546875" style="261" customWidth="1"/>
+    <col min="30" max="30" width="19.44140625" style="261" customWidth="1"/>
+    <col min="31" max="31" width="17.5546875" style="261" customWidth="1"/>
+    <col min="32" max="32" width="17.5546875" style="368" customWidth="1"/>
+    <col min="33" max="33" width="22.44140625" style="261" customWidth="1"/>
+    <col min="34" max="34" width="12.5546875" style="261" customWidth="1"/>
+    <col min="35" max="35" width="18.44140625" style="262" customWidth="1"/>
+    <col min="36" max="36" width="20.88671875" style="261" customWidth="1"/>
+    <col min="37" max="37" width="12.88671875" style="261" customWidth="1"/>
+    <col min="38" max="38" width="13.5546875" style="261" customWidth="1"/>
+    <col min="39" max="39" width="16.5546875" style="261" customWidth="1"/>
+    <col min="40" max="40" width="13.88671875" style="261" customWidth="1"/>
+    <col min="41" max="41" width="19.109375" style="261" customWidth="1"/>
+    <col min="42" max="42" width="16.5546875" style="261" customWidth="1"/>
+    <col min="43" max="43" width="14.5546875" style="261" customWidth="1"/>
+    <col min="44" max="44" width="14.88671875" style="261" customWidth="1"/>
+    <col min="45" max="45" width="15.44140625" style="261" customWidth="1"/>
     <col min="46" max="46" width="16" style="261" customWidth="1"/>
-    <col min="47" max="47" width="16.5703125" style="261" customWidth="1"/>
-    <col min="48" max="48" width="12.42578125" style="261" customWidth="1"/>
-    <col min="49" max="49" width="8.7109375" style="261"/>
-    <col min="50" max="50" width="17.5703125" style="358" customWidth="1"/>
-    <col min="51" max="51" width="16.42578125" style="358" customWidth="1"/>
-    <col min="52" max="52" width="15.28515625" style="380" customWidth="1"/>
-    <col min="53" max="53" width="16.5703125" style="358" customWidth="1"/>
+    <col min="47" max="47" width="16.5546875" style="261" customWidth="1"/>
+    <col min="48" max="48" width="12.44140625" style="261" customWidth="1"/>
+    <col min="49" max="49" width="8.6640625" style="261"/>
+    <col min="50" max="50" width="17.5546875" style="358" customWidth="1"/>
+    <col min="51" max="51" width="16.44140625" style="358" customWidth="1"/>
+    <col min="52" max="52" width="15.33203125" style="380" customWidth="1"/>
+    <col min="53" max="53" width="16.5546875" style="358" customWidth="1"/>
     <col min="54" max="54" width="16" style="358" customWidth="1"/>
     <col min="55" max="55" width="18" style="358" customWidth="1"/>
-    <col min="56" max="56" width="14.42578125" style="362" customWidth="1"/>
-    <col min="57" max="57" width="16.5703125" style="358" customWidth="1"/>
-    <col min="58" max="58" width="13.140625" style="358" customWidth="1"/>
-    <col min="59" max="59" width="14.42578125" style="362" customWidth="1"/>
-    <col min="60" max="60" width="13.5703125" style="362" customWidth="1"/>
-    <col min="61" max="62" width="11.85546875" style="362" customWidth="1"/>
-    <col min="63" max="63" width="12.42578125" style="362" customWidth="1"/>
-    <col min="64" max="64" width="12.85546875" style="362" customWidth="1"/>
-    <col min="65" max="66" width="13.42578125" style="362" customWidth="1"/>
-    <col min="67" max="16384" width="8.7109375" style="261"/>
+    <col min="56" max="56" width="14.44140625" style="362" customWidth="1"/>
+    <col min="57" max="57" width="16.5546875" style="358" customWidth="1"/>
+    <col min="58" max="58" width="13.109375" style="358" customWidth="1"/>
+    <col min="59" max="59" width="14.44140625" style="362" customWidth="1"/>
+    <col min="60" max="60" width="13.5546875" style="362" customWidth="1"/>
+    <col min="61" max="62" width="11.88671875" style="362" customWidth="1"/>
+    <col min="63" max="63" width="12.44140625" style="362" customWidth="1"/>
+    <col min="64" max="64" width="12.88671875" style="362" customWidth="1"/>
+    <col min="65" max="66" width="13.44140625" style="362" customWidth="1"/>
+    <col min="67" max="16384" width="8.6640625" style="261"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="23.25">
+    <row r="1" spans="1:74" ht="22.8">
       <c r="A1" s="260"/>
       <c r="B1" s="514" t="s">
         <v>93</v>
@@ -23044,7 +23041,7 @@
       <c r="BF1" s="515"/>
       <c r="BG1" s="515"/>
     </row>
-    <row r="2" spans="1:74" s="349" customFormat="1" ht="25.5">
+    <row r="2" spans="1:74" s="349" customFormat="1" ht="26.4">
       <c r="C2" s="350" t="s">
         <v>94</v>
       </c>
@@ -23194,7 +23191,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="356" customFormat="1" ht="63.75">
+    <row r="3" spans="1:74" s="356" customFormat="1" ht="66">
       <c r="A3" s="356" t="s">
         <v>1752</v>
       </c>
@@ -23568,7 +23565,7 @@
       <c r="BS4" s="355"/>
       <c r="BT4" s="355"/>
     </row>
-    <row r="5" spans="1:74" s="266" customFormat="1" ht="240">
+    <row r="5" spans="1:74" s="266" customFormat="1" ht="216">
       <c r="A5" s="263" t="s">
         <v>163</v>
       </c>
@@ -23772,7 +23769,7 @@
       <c r="BS5" s="265"/>
       <c r="BT5" s="265"/>
     </row>
-    <row r="6" spans="1:74" s="459" customFormat="1" ht="41.45" customHeight="1">
+    <row r="6" spans="1:74" s="459" customFormat="1" ht="41.4" customHeight="1">
       <c r="A6" s="452" t="s">
         <v>201</v>
       </c>
@@ -24045,7 +24042,7 @@
       <c r="BM7" s="364"/>
       <c r="BN7" s="364"/>
     </row>
-    <row r="8" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="8" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A8" s="267" t="s">
         <v>232</v>
       </c>
@@ -24153,7 +24150,7 @@
       <c r="BM8" s="364"/>
       <c r="BN8" s="364"/>
     </row>
-    <row r="9" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="9" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A9" s="267" t="s">
         <v>235</v>
       </c>
@@ -24259,7 +24256,7 @@
       <c r="BM9" s="364"/>
       <c r="BN9" s="364"/>
     </row>
-    <row r="10" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="10" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A10" s="267" t="s">
         <v>236</v>
       </c>
@@ -24368,7 +24365,7 @@
       <c r="BM10" s="364"/>
       <c r="BN10" s="364"/>
     </row>
-    <row r="11" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="11" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A11" s="267" t="s">
         <v>238</v>
       </c>
@@ -24478,7 +24475,7 @@
       <c r="BM11" s="364"/>
       <c r="BN11" s="364"/>
     </row>
-    <row r="12" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="12" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A12" s="267" t="s">
         <v>246</v>
       </c>
@@ -24587,7 +24584,7 @@
       <c r="BM12" s="364"/>
       <c r="BN12" s="364"/>
     </row>
-    <row r="13" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="13" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A13" s="267" t="s">
         <v>247</v>
       </c>
@@ -24693,7 +24690,7 @@
       <c r="BM13" s="364"/>
       <c r="BN13" s="364"/>
     </row>
-    <row r="14" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="14" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A14" s="267" t="s">
         <v>248</v>
       </c>
@@ -24803,7 +24800,7 @@
       <c r="BM14" s="364"/>
       <c r="BN14" s="364"/>
     </row>
-    <row r="15" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="15" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A15" s="267" t="s">
         <v>251</v>
       </c>
@@ -24906,7 +24903,7 @@
       <c r="BM15" s="364"/>
       <c r="BN15" s="364"/>
     </row>
-    <row r="16" spans="1:74" s="268" customFormat="1" ht="33.75">
+    <row r="16" spans="1:74" s="268" customFormat="1" ht="32.4">
       <c r="A16" s="267" t="s">
         <v>252</v>
       </c>
@@ -25015,7 +25012,7 @@
       <c r="BM16" s="364"/>
       <c r="BN16" s="364"/>
     </row>
-    <row r="17" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="17" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A17" s="267" t="s">
         <v>254</v>
       </c>
@@ -25124,7 +25121,7 @@
       <c r="BM17" s="364"/>
       <c r="BN17" s="364"/>
     </row>
-    <row r="18" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="18" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A18" s="267" t="s">
         <v>256</v>
       </c>
@@ -25230,7 +25227,7 @@
       <c r="BM18" s="364"/>
       <c r="BN18" s="364"/>
     </row>
-    <row r="19" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="19" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A19" s="267" t="s">
         <v>257</v>
       </c>
@@ -25337,7 +25334,7 @@
       <c r="BM19" s="364"/>
       <c r="BN19" s="364"/>
     </row>
-    <row r="20" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="20" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A20" s="267" t="s">
         <v>259</v>
       </c>
@@ -25447,7 +25444,7 @@
       <c r="BM20" s="364"/>
       <c r="BN20" s="364"/>
     </row>
-    <row r="21" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="21" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A21" s="267" t="s">
         <v>262</v>
       </c>
@@ -25553,7 +25550,7 @@
       <c r="BM21" s="364"/>
       <c r="BN21" s="364"/>
     </row>
-    <row r="22" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="22" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A22" s="267" t="s">
         <v>264</v>
       </c>
@@ -25662,7 +25659,7 @@
       <c r="BM22" s="364"/>
       <c r="BN22" s="364"/>
     </row>
-    <row r="23" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="23" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A23" s="267" t="s">
         <v>265</v>
       </c>
@@ -25769,7 +25766,7 @@
       <c r="BM23" s="364"/>
       <c r="BN23" s="364"/>
     </row>
-    <row r="24" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="24" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A24" s="267" t="s">
         <v>267</v>
       </c>
@@ -25878,7 +25875,7 @@
       <c r="BM24" s="364"/>
       <c r="BN24" s="364"/>
     </row>
-    <row r="25" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="25" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A25" s="267" t="s">
         <v>268</v>
       </c>
@@ -25984,7 +25981,7 @@
       <c r="BM25" s="364"/>
       <c r="BN25" s="364"/>
     </row>
-    <row r="26" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="26" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A26" s="267" t="s">
         <v>269</v>
       </c>
@@ -26093,7 +26090,7 @@
       <c r="BM26" s="364"/>
       <c r="BN26" s="364"/>
     </row>
-    <row r="27" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="27" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A27" s="267" t="s">
         <v>270</v>
       </c>
@@ -26200,7 +26197,7 @@
       <c r="BM27" s="364"/>
       <c r="BN27" s="364"/>
     </row>
-    <row r="28" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="28" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A28" s="267" t="s">
         <v>273</v>
       </c>
@@ -26305,7 +26302,7 @@
       </c>
       <c r="BN28" s="364"/>
     </row>
-    <row r="29" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="29" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A29" s="267" t="s">
         <v>277</v>
       </c>
@@ -26408,7 +26405,7 @@
       <c r="BM29" s="364"/>
       <c r="BN29" s="364"/>
     </row>
-    <row r="30" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="30" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A30" s="267" t="s">
         <v>278</v>
       </c>
@@ -26515,7 +26512,7 @@
       <c r="BM30" s="364"/>
       <c r="BN30" s="364"/>
     </row>
-    <row r="31" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="31" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A31" s="267" t="s">
         <v>280</v>
       </c>
@@ -26621,7 +26618,7 @@
       <c r="BM31" s="364"/>
       <c r="BN31" s="364"/>
     </row>
-    <row r="32" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="32" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A32" s="267" t="s">
         <v>281</v>
       </c>
@@ -26730,7 +26727,7 @@
       <c r="BM32" s="364"/>
       <c r="BN32" s="364"/>
     </row>
-    <row r="33" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="33" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A33" s="267" t="s">
         <v>282</v>
       </c>
@@ -26838,7 +26835,7 @@
       <c r="BM33" s="364"/>
       <c r="BN33" s="364"/>
     </row>
-    <row r="34" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="34" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A34" s="267" t="s">
         <v>285</v>
       </c>
@@ -26944,7 +26941,7 @@
       <c r="BM34" s="364"/>
       <c r="BN34" s="364"/>
     </row>
-    <row r="35" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="35" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A35" s="267" t="s">
         <v>286</v>
       </c>
@@ -27051,7 +27048,7 @@
       <c r="BM35" s="364"/>
       <c r="BN35" s="364"/>
     </row>
-    <row r="36" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="36" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A36" s="267" t="s">
         <v>288</v>
       </c>
@@ -27160,7 +27157,7 @@
       <c r="BM36" s="364"/>
       <c r="BN36" s="364"/>
     </row>
-    <row r="37" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="37" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A37" s="267" t="s">
         <v>290</v>
       </c>
@@ -27270,7 +27267,7 @@
       <c r="BM37" s="364"/>
       <c r="BN37" s="364"/>
     </row>
-    <row r="38" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="38" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A38" s="267" t="s">
         <v>293</v>
       </c>
@@ -27376,7 +27373,7 @@
       <c r="BM38" s="364"/>
       <c r="BN38" s="364"/>
     </row>
-    <row r="39" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="39" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A39" s="267" t="s">
         <v>294</v>
       </c>
@@ -27494,7 +27491,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="40" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A40" s="267" t="s">
         <v>307</v>
       </c>
@@ -27600,7 +27597,7 @@
       <c r="BM40" s="364"/>
       <c r="BN40" s="364"/>
     </row>
-    <row r="41" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="41" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A41" s="267" t="s">
         <v>308</v>
       </c>
@@ -27702,7 +27699,7 @@
       <c r="BM41" s="364"/>
       <c r="BN41" s="364"/>
     </row>
-    <row r="42" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="42" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A42" s="267" t="s">
         <v>309</v>
       </c>
@@ -27811,7 +27808,7 @@
       <c r="BM42" s="364"/>
       <c r="BN42" s="364"/>
     </row>
-    <row r="43" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="43" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A43" s="267" t="s">
         <v>310</v>
       </c>
@@ -27920,7 +27917,7 @@
       <c r="BM43" s="364"/>
       <c r="BN43" s="364"/>
     </row>
-    <row r="44" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="44" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A44" s="267" t="s">
         <v>312</v>
       </c>
@@ -28026,7 +28023,7 @@
       <c r="BM44" s="364"/>
       <c r="BN44" s="364"/>
     </row>
-    <row r="45" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="45" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A45" s="267" t="s">
         <v>313</v>
       </c>
@@ -28132,7 +28129,7 @@
       <c r="BM45" s="364"/>
       <c r="BN45" s="364"/>
     </row>
-    <row r="46" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="46" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A46" s="267" t="s">
         <v>315</v>
       </c>
@@ -28241,7 +28238,7 @@
       <c r="BM46" s="364"/>
       <c r="BN46" s="364"/>
     </row>
-    <row r="47" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="47" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A47" s="267" t="s">
         <v>316</v>
       </c>
@@ -28346,7 +28343,7 @@
       <c r="BM47" s="364"/>
       <c r="BN47" s="364"/>
     </row>
-    <row r="48" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="48" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A48" s="267" t="s">
         <v>317</v>
       </c>
@@ -28452,7 +28449,7 @@
       <c r="BM48" s="364"/>
       <c r="BN48" s="364"/>
     </row>
-    <row r="49" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="49" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A49" s="267" t="s">
         <v>318</v>
       </c>
@@ -28558,7 +28555,7 @@
       <c r="BM49" s="364"/>
       <c r="BN49" s="364"/>
     </row>
-    <row r="50" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="50" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A50" s="267" t="s">
         <v>320</v>
       </c>
@@ -28667,7 +28664,7 @@
       <c r="BM50" s="364"/>
       <c r="BN50" s="364"/>
     </row>
-    <row r="51" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="51" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A51" s="267" t="s">
         <v>321</v>
       </c>
@@ -28776,7 +28773,7 @@
       <c r="BM51" s="364"/>
       <c r="BN51" s="364"/>
     </row>
-    <row r="52" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="52" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A52" s="267" t="s">
         <v>322</v>
       </c>
@@ -28881,7 +28878,7 @@
       <c r="BM52" s="364"/>
       <c r="BN52" s="364"/>
     </row>
-    <row r="53" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="53" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A53" s="267" t="s">
         <v>73</v>
       </c>
@@ -28990,7 +28987,7 @@
       <c r="BM53" s="364"/>
       <c r="BN53" s="364"/>
     </row>
-    <row r="54" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="54" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A54" s="267" t="s">
         <v>323</v>
       </c>
@@ -29097,7 +29094,7 @@
       <c r="BM54" s="364"/>
       <c r="BN54" s="364"/>
     </row>
-    <row r="55" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="55" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A55" s="267" t="s">
         <v>325</v>
       </c>
@@ -29206,7 +29203,7 @@
       <c r="BM55" s="364"/>
       <c r="BN55" s="364"/>
     </row>
-    <row r="56" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="56" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A56" s="267" t="s">
         <v>326</v>
       </c>
@@ -29315,7 +29312,7 @@
       <c r="BM56" s="364"/>
       <c r="BN56" s="364"/>
     </row>
-    <row r="57" spans="1:66" s="268" customFormat="1" ht="33.75">
+    <row r="57" spans="1:66" s="268" customFormat="1" ht="32.4">
       <c r="A57" s="267" t="s">
         <v>327</v>
       </c>
@@ -29828,11 +29825,11 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29935,59 +29932,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870F3D7E-D500-4249-A60B-8D4257022104}">
   <dimension ref="A1:AZ205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AH98" sqref="AH98"/>
+      <selection pane="bottomLeft" activeCell="AI98" sqref="AI98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="104.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" customWidth="1"/>
-    <col min="16" max="16" width="22.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="25.28515625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" customWidth="1"/>
-    <col min="22" max="25" width="19.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="37.109375" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="25.33203125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="25.88671875" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" customWidth="1"/>
+    <col min="22" max="25" width="19.109375" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="22" customWidth="1"/>
-    <col min="27" max="27" width="8.5703125" customWidth="1"/>
+    <col min="27" max="27" width="8.5546875" customWidth="1"/>
     <col min="28" max="28" width="3" customWidth="1"/>
-    <col min="29" max="30" width="3.28515625" customWidth="1"/>
-    <col min="31" max="31" width="16.28515625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="8.140625" customWidth="1"/>
-    <col min="33" max="33" width="25.140625" customWidth="1"/>
-    <col min="34" max="34" width="48.28515625" style="463" customWidth="1"/>
-    <col min="35" max="35" width="83.85546875" customWidth="1"/>
-    <col min="36" max="36" width="8.28515625" customWidth="1"/>
-    <col min="37" max="37" width="8.140625" customWidth="1"/>
-    <col min="38" max="38" width="9.140625" customWidth="1"/>
-    <col min="39" max="40" width="8.42578125" customWidth="1"/>
-    <col min="41" max="41" width="9.42578125" customWidth="1"/>
-    <col min="42" max="42" width="40.85546875" customWidth="1"/>
-    <col min="43" max="43" width="7.5703125" customWidth="1"/>
-    <col min="44" max="44" width="5.140625" customWidth="1"/>
-    <col min="45" max="45" width="24.5703125" customWidth="1"/>
-    <col min="46" max="47" width="7.5703125" customWidth="1"/>
-    <col min="48" max="48" width="23.85546875" customWidth="1"/>
-    <col min="49" max="49" width="18.42578125" customWidth="1"/>
-    <col min="50" max="50" width="41.85546875" customWidth="1"/>
-    <col min="51" max="51" width="65.140625" style="196" customWidth="1"/>
+    <col min="29" max="30" width="3.33203125" customWidth="1"/>
+    <col min="31" max="31" width="16.33203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="8.109375" customWidth="1"/>
+    <col min="33" max="33" width="25.109375" customWidth="1"/>
+    <col min="34" max="34" width="48.33203125" style="463" customWidth="1"/>
+    <col min="35" max="35" width="83.88671875" customWidth="1"/>
+    <col min="36" max="36" width="8.33203125" customWidth="1"/>
+    <col min="37" max="37" width="8.109375" customWidth="1"/>
+    <col min="38" max="38" width="9.109375" customWidth="1"/>
+    <col min="39" max="40" width="8.44140625" customWidth="1"/>
+    <col min="41" max="41" width="9.44140625" customWidth="1"/>
+    <col min="42" max="42" width="40.88671875" customWidth="1"/>
+    <col min="43" max="43" width="7.5546875" customWidth="1"/>
+    <col min="44" max="44" width="5.109375" customWidth="1"/>
+    <col min="45" max="45" width="24.5546875" customWidth="1"/>
+    <col min="46" max="47" width="7.5546875" customWidth="1"/>
+    <col min="48" max="48" width="23.88671875" customWidth="1"/>
+    <col min="49" max="49" width="18.44140625" customWidth="1"/>
+    <col min="50" max="50" width="41.88671875" customWidth="1"/>
+    <col min="51" max="51" width="65.109375" style="196" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="33" customHeight="1">
@@ -32839,7 +32836,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="24" spans="1:51" ht="165">
+    <row r="24" spans="1:51" ht="165.6">
       <c r="A24" s="76" t="s">
         <v>2102</v>
       </c>
@@ -32964,7 +32961,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="25" spans="1:51" ht="165">
+    <row r="25" spans="1:51" ht="144">
       <c r="A25" s="76" t="s">
         <v>2102</v>
       </c>
@@ -33089,7 +33086,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="26" spans="1:51" ht="165">
+    <row r="26" spans="1:51" ht="144">
       <c r="A26" s="76" t="s">
         <v>2102</v>
       </c>
@@ -33214,7 +33211,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="27" spans="1:51" ht="165">
+    <row r="27" spans="1:51" ht="144">
       <c r="A27" s="76" t="s">
         <v>2102</v>
       </c>
@@ -33339,7 +33336,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="28" spans="1:51" ht="90">
+    <row r="28" spans="1:51" ht="86.4">
       <c r="A28" s="76" t="s">
         <v>2102</v>
       </c>
@@ -35063,7 +35060,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="42" spans="1:51" ht="135">
+    <row r="42" spans="1:51" ht="138">
       <c r="A42" s="76" t="s">
         <v>2102</v>
       </c>
@@ -35186,7 +35183,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="43" spans="1:51" s="193" customFormat="1" ht="108">
+    <row r="43" spans="1:51" s="193" customFormat="1" ht="124.2">
       <c r="A43" s="288" t="s">
         <v>2102</v>
       </c>
@@ -35908,7 +35905,7 @@
       <c r="AX48" s="414"/>
       <c r="AY48" s="420"/>
     </row>
-    <row r="49" spans="1:51" ht="175.5">
+    <row r="49" spans="1:51" ht="179.4">
       <c r="A49" s="76" t="s">
         <v>2102</v>
       </c>
@@ -36031,7 +36028,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="50" spans="1:51" ht="162">
+    <row r="50" spans="1:51" ht="179.4">
       <c r="A50" s="76" t="s">
         <v>2102</v>
       </c>
@@ -36156,7 +36153,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="51" spans="1:51" ht="175.5">
+    <row r="51" spans="1:51" ht="179.4">
       <c r="A51" s="76" t="s">
         <v>2102</v>
       </c>
@@ -36281,7 +36278,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="52" spans="1:51" ht="162">
+    <row r="52" spans="1:51" ht="165.6">
       <c r="A52" s="76" t="s">
         <v>2102</v>
       </c>
@@ -36406,7 +36403,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="53" spans="1:51" ht="175.5">
+    <row r="53" spans="1:51" ht="179.4">
       <c r="A53" s="76" t="s">
         <v>2102</v>
       </c>
@@ -38094,7 +38091,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="67" spans="1:51" s="115" customFormat="1" ht="108">
+    <row r="67" spans="1:51" s="115" customFormat="1" ht="110.4">
       <c r="A67" s="220" t="s">
         <v>2102</v>
       </c>
@@ -39116,10 +39113,10 @@
       </c>
       <c r="AF75" s="221"/>
       <c r="AG75" s="111" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="AH75" s="461" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="AI75" s="151" t="s">
         <v>2364</v>
@@ -39227,10 +39224,10 @@
       </c>
       <c r="AF76" s="221"/>
       <c r="AG76" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH76" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH76" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI76" s="151" t="s">
         <v>2366</v>
@@ -39334,10 +39331,10 @@
       </c>
       <c r="AF77" s="221"/>
       <c r="AG77" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH77" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH77" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI77" s="108" t="s">
         <v>2367</v>
@@ -39439,10 +39436,10 @@
       </c>
       <c r="AF78" s="221"/>
       <c r="AG78" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH78" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH78" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI78" s="335"/>
       <c r="AJ78" s="110"/>
@@ -39544,10 +39541,10 @@
       </c>
       <c r="AF79" s="221"/>
       <c r="AG79" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH79" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH79" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI79" s="108" t="s">
         <v>2368</v>
@@ -39651,10 +39648,10 @@
       </c>
       <c r="AF80" s="221"/>
       <c r="AG80" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH80" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH80" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI80" s="108" t="s">
         <v>2369</v>
@@ -39694,7 +39691,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="109" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="D81" s="141" t="s">
         <v>26</v>
@@ -39760,10 +39757,10 @@
       </c>
       <c r="AF81" s="221"/>
       <c r="AG81" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH81" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH81" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI81" s="108" t="s">
         <v>2370</v>
@@ -39867,10 +39864,10 @@
       </c>
       <c r="AF82" s="221"/>
       <c r="AG82" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH82" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH82" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI82" s="108" t="s">
         <v>2371</v>
@@ -39974,10 +39971,10 @@
       </c>
       <c r="AF83" s="221"/>
       <c r="AG83" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH83" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH83" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI83" s="108" t="s">
         <v>2372</v>
@@ -40087,10 +40084,10 @@
       </c>
       <c r="AF84" s="221"/>
       <c r="AG84" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH84" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH84" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI84" s="151" t="s">
         <v>2373</v>
@@ -40196,10 +40193,10 @@
       </c>
       <c r="AF85" s="341"/>
       <c r="AG85" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH85" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH85" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI85" s="108" t="s">
         <v>2374</v>
@@ -40301,10 +40298,10 @@
       </c>
       <c r="AF86" s="109"/>
       <c r="AG86" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH86" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH86" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI86" s="108"/>
       <c r="AJ86" s="110"/>
@@ -40400,17 +40397,17 @@
         <v>387</v>
       </c>
       <c r="AE87" s="109" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="AF87" s="109"/>
       <c r="AG87" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH87" s="461" t="s">
         <v>2388</v>
       </c>
-      <c r="AH87" s="461" t="s">
-        <v>2389</v>
-      </c>
       <c r="AI87" s="108" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="AJ87" s="110"/>
       <c r="AK87" s="166">
@@ -40513,10 +40510,10 @@
       </c>
       <c r="AF88" s="109"/>
       <c r="AG88" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH88" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH88" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI88" s="108" t="s">
         <v>2376</v>
@@ -40622,10 +40619,10 @@
       </c>
       <c r="AF89" s="109"/>
       <c r="AG89" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH89" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH89" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI89" s="108" t="s">
         <v>2378</v>
@@ -40731,10 +40728,10 @@
       </c>
       <c r="AF90" s="109"/>
       <c r="AG90" s="111" t="s">
+        <v>2396</v>
+      </c>
+      <c r="AH90" s="461" t="s">
         <v>2397</v>
-      </c>
-      <c r="AH90" s="461" t="s">
-        <v>2398</v>
       </c>
       <c r="AI90" s="108" t="s">
         <v>2380</v>
@@ -40836,10 +40833,10 @@
       </c>
       <c r="AF91" s="109"/>
       <c r="AG91" s="111" t="s">
+        <v>2396</v>
+      </c>
+      <c r="AH91" s="461" t="s">
         <v>2397</v>
-      </c>
-      <c r="AH91" s="461" t="s">
-        <v>2398</v>
       </c>
       <c r="AI91" s="108" t="s">
         <v>2381</v>
@@ -40941,10 +40938,10 @@
       </c>
       <c r="AF92" s="109"/>
       <c r="AG92" s="111" t="s">
+        <v>2396</v>
+      </c>
+      <c r="AH92" s="461" t="s">
         <v>2397</v>
-      </c>
-      <c r="AH92" s="461" t="s">
-        <v>2398</v>
       </c>
       <c r="AI92" s="108" t="s">
         <v>2382</v>
@@ -41046,10 +41043,10 @@
       </c>
       <c r="AF93" s="109"/>
       <c r="AG93" s="111" t="s">
+        <v>2396</v>
+      </c>
+      <c r="AH93" s="461" t="s">
         <v>2397</v>
-      </c>
-      <c r="AH93" s="461" t="s">
-        <v>2398</v>
       </c>
       <c r="AI93" s="108" t="s">
         <v>2383</v>
@@ -41151,10 +41148,10 @@
       </c>
       <c r="AF94" s="109"/>
       <c r="AG94" s="111" t="s">
+        <v>2396</v>
+      </c>
+      <c r="AH94" s="461" t="s">
         <v>2397</v>
-      </c>
-      <c r="AH94" s="461" t="s">
-        <v>2398</v>
       </c>
       <c r="AI94" s="108" t="s">
         <v>2384</v>
@@ -41254,10 +41251,10 @@
       </c>
       <c r="AF95" s="109"/>
       <c r="AG95" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH95" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH95" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI95" s="335" t="s">
         <v>539</v>
@@ -41355,17 +41352,17 @@
         <v>387</v>
       </c>
       <c r="AE96" s="109" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="AF96" s="109"/>
       <c r="AG96" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH96" s="461" t="s">
         <v>2388</v>
       </c>
-      <c r="AH96" s="461" t="s">
-        <v>2389</v>
-      </c>
       <c r="AI96" s="108" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="AJ96" s="110"/>
       <c r="AK96" s="107" t="s">
@@ -41460,17 +41457,17 @@
         <v>387</v>
       </c>
       <c r="AE97" s="109" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="AF97" s="109"/>
       <c r="AG97" s="111" t="s">
+        <v>2400</v>
+      </c>
+      <c r="AH97" s="461" t="s">
         <v>2401</v>
       </c>
-      <c r="AH97" s="461" t="s">
-        <v>2402</v>
-      </c>
       <c r="AI97" s="108" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="AJ97" s="110"/>
       <c r="AK97" s="107" t="s">
@@ -41569,10 +41566,10 @@
       </c>
       <c r="AF98" s="109"/>
       <c r="AG98" s="111" t="s">
+        <v>2387</v>
+      </c>
+      <c r="AH98" s="461" t="s">
         <v>2388</v>
-      </c>
-      <c r="AH98" s="461" t="s">
-        <v>2389</v>
       </c>
       <c r="AI98" s="108" t="s">
         <v>2386</v>
@@ -41674,13 +41671,13 @@
       </c>
       <c r="AF99" s="109"/>
       <c r="AG99" s="111" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="AH99" s="461" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="AI99" s="151" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="AJ99" s="110"/>
       <c r="AK99" s="508" t="s">
@@ -41779,13 +41776,13 @@
       </c>
       <c r="AF100" s="109"/>
       <c r="AG100" s="111" t="s">
+        <v>2390</v>
+      </c>
+      <c r="AH100" s="461" t="s">
         <v>2391</v>
       </c>
-      <c r="AH100" s="461" t="s">
-        <v>2392</v>
-      </c>
       <c r="AI100" s="151" t="s">
-        <v>2387</v>
+        <v>2404</v>
       </c>
       <c r="AJ100" s="110"/>
       <c r="AK100" s="107" t="s">
@@ -53025,53 +53022,53 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="115" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="115" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.140625" customWidth="1"/>
-    <col min="20" max="20" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.109375" customWidth="1"/>
+    <col min="20" max="20" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="28.28515625" customWidth="1"/>
-    <col min="23" max="24" width="26.85546875" style="168" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="21.28515625" customWidth="1"/>
-    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.33203125" customWidth="1"/>
+    <col min="23" max="24" width="26.88671875" style="168" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="21.33203125" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="25.140625" customWidth="1"/>
-    <col min="31" max="31" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.28515625" customWidth="1"/>
-    <col min="33" max="33" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.140625" customWidth="1"/>
+    <col min="30" max="30" width="25.109375" customWidth="1"/>
+    <col min="31" max="31" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.33203125" customWidth="1"/>
+    <col min="33" max="33" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.109375" customWidth="1"/>
     <col min="36" max="36" width="18" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.85546875" customWidth="1"/>
-    <col min="38" max="38" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="28.28515625" customWidth="1"/>
-    <col min="40" max="40" width="25.5703125" customWidth="1"/>
-    <col min="41" max="41" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" customWidth="1"/>
-    <col min="43" max="43" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="24.140625" customWidth="1"/>
-    <col min="45" max="45" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.88671875" customWidth="1"/>
+    <col min="38" max="38" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.33203125" customWidth="1"/>
+    <col min="40" max="40" width="25.5546875" customWidth="1"/>
+    <col min="41" max="41" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5546875" customWidth="1"/>
+    <col min="43" max="43" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.109375" customWidth="1"/>
+    <col min="45" max="45" width="32.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="475" customFormat="1" ht="75">
+    <row r="1" spans="1:51" s="475" customFormat="1" ht="72">
       <c r="A1" s="472" t="s">
         <v>1065</v>
       </c>
@@ -53214,7 +53211,7 @@
       <c r="AX1" s="474"/>
       <c r="AY1" s="474"/>
     </row>
-    <row r="2" spans="1:51" s="478" customFormat="1" ht="18.75">
+    <row r="2" spans="1:51" s="478" customFormat="1" ht="18">
       <c r="A2" s="476" t="s">
         <v>375</v>
       </c>
@@ -53351,7 +53348,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:51" s="86" customFormat="1" ht="90">
+    <row r="3" spans="1:51" s="86" customFormat="1" ht="72">
       <c r="A3" s="81" t="s">
         <v>1096</v>
       </c>
@@ -53488,7 +53485,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="4" spans="1:51" s="86" customFormat="1" ht="90">
+    <row r="4" spans="1:51" s="86" customFormat="1" ht="86.4">
       <c r="A4" s="81" t="s">
         <v>1123</v>
       </c>
@@ -53619,7 +53616,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="5" spans="1:51" s="86" customFormat="1" ht="90">
+    <row r="5" spans="1:51" s="86" customFormat="1" ht="86.4">
       <c r="A5" s="81" t="s">
         <v>1145</v>
       </c>
@@ -53716,7 +53713,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="6" spans="1:51" s="86" customFormat="1" ht="90">
+    <row r="6" spans="1:51" s="86" customFormat="1" ht="72">
       <c r="A6" s="81" t="s">
         <v>1162</v>
       </c>
@@ -53783,7 +53780,7 @@
       </c>
       <c r="AR6" s="81"/>
     </row>
-    <row r="7" spans="1:51" s="86" customFormat="1" ht="75">
+    <row r="7" spans="1:51" s="86" customFormat="1" ht="72">
       <c r="A7" s="81" t="s">
         <v>1172</v>
       </c>
@@ -56378,12 +56375,12 @@
       <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="34.5" customHeight="1">
@@ -56405,7 +56402,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="259" customFormat="1" ht="60">
+    <row r="3" spans="1:4" s="259" customFormat="1" ht="57.6">
       <c r="A3" s="273" t="s">
         <v>1489</v>
       </c>
@@ -56419,7 +56416,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="259" customFormat="1" ht="60">
+    <row r="4" spans="1:4" s="259" customFormat="1" ht="57.6">
       <c r="A4" s="273" t="s">
         <v>1489</v>
       </c>
@@ -56433,7 +56430,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="75" customFormat="1" ht="45">
+    <row r="5" spans="1:4" s="75" customFormat="1" ht="28.8">
       <c r="A5" s="103" t="s">
         <v>1495</v>
       </c>
@@ -56442,7 +56439,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60">
+    <row r="6" spans="1:4" ht="57.6">
       <c r="A6" s="81" t="s">
         <v>1497</v>
       </c>
@@ -56451,7 +56448,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60">
+    <row r="7" spans="1:4" ht="57.6">
       <c r="A7" s="81" t="s">
         <v>1499</v>
       </c>
@@ -56460,7 +56457,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="75" customFormat="1" ht="30">
+    <row r="8" spans="1:4" s="75" customFormat="1" ht="28.8">
       <c r="A8" s="103" t="s">
         <v>1501</v>
       </c>
@@ -56543,7 +56540,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="28.8">
       <c r="A24" s="242" t="s">
         <v>1779</v>
       </c>
@@ -56556,7 +56553,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="45">
+    <row r="57" spans="1:5" ht="43.2">
       <c r="A57" s="103" t="s">
         <v>1783</v>
       </c>
@@ -56565,7 +56562,7 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="45">
+    <row r="58" spans="1:5" ht="28.8">
       <c r="A58" s="103" t="s">
         <v>1785</v>
       </c>
@@ -56706,16 +56703,16 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
     <col min="6" max="6" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="48.75" thickTop="1" thickBot="1">
+    <row r="1" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A1" s="197" t="s">
         <v>1512</v>
       </c>
@@ -56735,7 +56732,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A2" s="517" t="s">
         <v>1091</v>
       </c>
@@ -56755,7 +56752,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="3" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A3" s="517"/>
       <c r="B3" s="200" t="s">
         <v>35</v>
@@ -56773,7 +56770,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="4" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A4" s="517"/>
       <c r="B4" s="200" t="s">
         <v>1161</v>
@@ -56791,7 +56788,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="5" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A5" s="206"/>
       <c r="B5" s="207"/>
       <c r="C5" s="213"/>
@@ -56799,7 +56796,7 @@
       <c r="E5" s="208"/>
       <c r="F5" s="207"/>
     </row>
-    <row r="6" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="6" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A6" s="517" t="s">
         <v>1118</v>
       </c>
@@ -56819,7 +56816,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="7" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A7" s="517"/>
       <c r="B7" s="200" t="s">
         <v>1121</v>
@@ -56837,7 +56834,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="8" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A8" s="517"/>
       <c r="B8" s="200" t="s">
         <v>35</v>
@@ -56855,7 +56852,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="9" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A9" s="517"/>
       <c r="B9" s="200" t="s">
         <v>1161</v>
@@ -56873,7 +56870,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="10" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A10" s="206"/>
       <c r="B10" s="207"/>
       <c r="C10" s="213"/>
@@ -56881,7 +56878,7 @@
       <c r="E10" s="209"/>
       <c r="F10" s="207"/>
     </row>
-    <row r="11" spans="1:6" ht="33" thickTop="1" thickBot="1">
+    <row r="11" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A11" s="517" t="s">
         <v>1159</v>
       </c>
@@ -56901,7 +56898,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="33" thickTop="1" thickBot="1">
+    <row r="12" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A12" s="517"/>
       <c r="B12" s="200" t="s">
         <v>1526</v>
@@ -56919,7 +56916,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="33" thickTop="1" thickBot="1">
+    <row r="13" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A13" s="517"/>
       <c r="B13" s="200" t="s">
         <v>1526</v>
@@ -56937,7 +56934,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="14" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A14" s="517"/>
       <c r="B14" s="200" t="s">
         <v>35</v>
@@ -56955,7 +56952,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="15" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A15" s="517"/>
       <c r="B15" s="200" t="s">
         <v>1161</v>
@@ -56973,7 +56970,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.25" thickTop="1" thickBot="1">
+    <row r="16" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
       <c r="A16" s="206"/>
       <c r="B16" s="207"/>
       <c r="C16" s="213"/>
@@ -56981,7 +56978,7 @@
       <c r="E16" s="207"/>
       <c r="F16" s="207"/>
     </row>
-    <row r="17" spans="1:6" ht="33" thickTop="1" thickBot="1">
+    <row r="17" spans="1:6" ht="32.4" thickTop="1" thickBot="1">
       <c r="A17" s="199" t="s">
         <v>1527</v>
       </c>
@@ -57001,7 +56998,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickTop="1"/>
+    <row r="18" spans="1:6" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A4"/>
@@ -57013,6 +57010,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9" xsi:nil="true"/>
+    <Created0 xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Choice_x002d_Test xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <Date xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <ClientNumber xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <PartitionCode xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
+      <UserInfo>
+        <DisplayName>Tammy Sunderland</DisplayName>
+        <AccountId>38</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A419301B98B8354A897828D82A6F00F6" ma:contentTypeVersion="34" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20ca8a0c0d59028efd0f33ef93e3a420">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3e08ed28-a208-4db3-90dc-062006ce0c78" xmlns:ns3="7e386c18-d449-4d9a-a5df-f64c6139a3c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ecc1aa61ba2aa3d92dc6750af3137611" ns2:_="" ns3:_="">
     <xsd:import namespace="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
@@ -57333,33 +57357,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9" xsi:nil="true"/>
-    <Created0 xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Choice_x002d_Test xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <Date xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <ClientNumber xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <PartitionCode xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
-      <UserInfo>
-        <DisplayName>Tammy Sunderland</DisplayName>
-        <AccountId>38</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -57370,6 +57367,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E841BFC-575E-4C80-B796-EDB398657E74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7e386c18-d449-4d9a-a5df-f64c6139a3c9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{827BF9C6-14B5-43FE-98BA-5537952370B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -57388,23 +57402,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E841BFC-575E-4C80-B796-EDB398657E74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7e386c18-d449-4d9a-a5df-f64c6139a3c9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BEDA91-E434-447E-A9AB-EB3F15901C97}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
change for handle <> opertor and trust module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Client/FILI.xlsx
+++ b/src/test/resources/testdata/Client/FILI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EC66DB-0AF9-47D1-B0C8-2939E1F9E97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDF53A7-AC93-43E0-BC98-E88AA1FCA6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" firstSheet="5" activeTab="5" xr2:uid="{8D0F94DE-3100-47E5-A17C-DB8B711FEBE7}"/>
   </bookViews>
@@ -13586,7 +13586,135 @@
     <cellStyle name="Normal 3 2" xfId="5" xr:uid="{50DE3D44-ABB6-42F7-A295-F0E77105A8F4}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="57">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -20829,73 +20957,73 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Z5:Z8">
-    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="38" priority="22" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",Z5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AA8">
-    <cfRule type="containsText" dxfId="23" priority="18" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",Z5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="19" operator="equal">
       <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z9:AA17">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",Z9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",Z9)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
       <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA8">
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",AA5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="O">
+    <cfRule type="containsText" dxfId="31" priority="23" operator="containsText" text="O">
       <formula>NOT(ISERROR(SEARCH("O",AA5)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="24" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA9:AA17">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="O">
+    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="O">
       <formula>NOT(ISERROR(SEARCH("O",AA9)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB17">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN9:AR17">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="O">
+    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="O">
       <formula>NOT(ISERROR(SEARCH("O",AN9)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",AN9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",AN9)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22044,24 +22172,24 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C5">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E5">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30173,10 +30301,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:E6">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30188,10 +30316,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870F3D7E-D500-4249-A60B-8D4257022104}">
   <dimension ref="A1:AZ203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="AA1" activePane="topRight" state="frozen"/>
       <selection activeCell="A332" sqref="A332"/>
-      <selection pane="topRight" activeCell="AH95" sqref="AH95"/>
+      <selection pane="topRight" activeCell="AH110" sqref="AH110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="104.25" customHeight="1"/>
@@ -53111,56 +53239,108 @@
   </sheetData>
   <autoFilter ref="A1:BD192" xr:uid="{870F3D7E-D500-4249-A60B-8D4257022104}"/>
   <phoneticPr fontId="78" type="noConversion"/>
-  <conditionalFormatting sqref="AB2:AC192">
-    <cfRule type="containsText" dxfId="40" priority="432" operator="containsText" text="N">
+  <conditionalFormatting sqref="AB2:AC100 AB148:AC192">
+    <cfRule type="containsText" dxfId="54" priority="446" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",AB2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="433" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="447" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="517" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="52" priority="531" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",AB2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC192">
-    <cfRule type="containsText" dxfId="37" priority="518" operator="containsText" text="O">
+  <conditionalFormatting sqref="AC2:AC100 AC148:AC192">
+    <cfRule type="containsText" dxfId="51" priority="532" operator="containsText" text="O">
       <formula>NOT(ISERROR(SEARCH("O",AC2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="533" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD192">
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
+  <conditionalFormatting sqref="AD2:AD100 AD148:AD192">
+    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="26" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="27" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD1048576">
-    <cfRule type="cellIs" dxfId="32" priority="104" operator="equal">
+  <conditionalFormatting sqref="AD2:AD100 AD148:AD1048576">
+    <cfRule type="cellIs" dxfId="46" priority="118" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ2:AU192">
-    <cfRule type="cellIs" dxfId="31" priority="69" operator="equal">
+  <conditionalFormatting sqref="AQ2:AU100 AQ148:AU192">
+    <cfRule type="cellIs" dxfId="45" priority="83" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="70" operator="containsText" text="O">
+    <cfRule type="containsText" dxfId="44" priority="84" operator="containsText" text="O">
       <formula>NOT(ISERROR(SEARCH("O",AQ2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="85" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="72" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="42" priority="86" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",AQ2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="73" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="41" priority="87" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",AQ2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB101:AC147">
+    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",AB101)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",AB101)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC101:AC147">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="O">
+      <formula>NOT(ISERROR(SEARCH("O",AC101)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD101:AD147">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD101:AD147">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ101:AU147">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="O">
+      <formula>NOT(ISERROR(SEARCH("O",AQ101)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",AQ101)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",AQ101)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -53169,7 +53349,7 @@
     <hyperlink ref="AL169" r:id="rId3" xr:uid="{B8A0C951-82C7-488B-A5EE-7CBF3669DC12}"/>
     <hyperlink ref="AL192" r:id="rId4" xr:uid="{BF7249AB-50A8-459E-BC72-C8FBDC96F7AD}"/>
     <hyperlink ref="AL74" r:id="rId5" xr:uid="{7F464BAD-E31B-441F-A3EA-8EEFEA69B63B}"/>
-    <hyperlink ref="AL147" r:id="rId6" xr:uid="{F392A321-4C55-4E4B-B7E4-3E1DD5082BBF}"/>
+    <hyperlink ref="AL147" r:id="rId6" xr:uid="{68AE26BC-5AB3-4ADE-8DAB-854715CAB58D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -56855,10 +57035,10 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="B66:D70">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -57182,12 +57362,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9" xsi:nil="true"/>
+    <Created0 xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Choice_x002d_Test xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <Date xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <ClientNumber xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <PartitionCode xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
+      <UserInfo>
+        <DisplayName>Tammy Sunderland</DisplayName>
+        <AccountId>38</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57512,36 +57710,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9" xsi:nil="true"/>
-    <Created0 xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Choice_x002d_Test xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <Date xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <ClientNumber xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <PartitionCode xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
-      <UserInfo>
-        <DisplayName>Tammy Sunderland</DisplayName>
-        <AccountId>38</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BEDA91-E434-447E-A9AB-EB3F15901C97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E841BFC-575E-4C80-B796-EDB398657E74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
+    <ds:schemaRef ds:uri="7e386c18-d449-4d9a-a5df-f64c6139a3c9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -57566,12 +57749,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E841BFC-575E-4C80-B796-EDB398657E74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BEDA91-E434-447E-A9AB-EB3F15901C97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
-    <ds:schemaRef ds:uri="7e386c18-d449-4d9a-a5df-f64c6139a3c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>